<commit_message>
Adicionando pasta e arquivos de documentação | 29.09.2024
</commit_message>
<xml_diff>
--- a/modelagem_banco_de_dados/esquema_de_tabelas.xlsx
+++ b/modelagem_banco_de_dados/esquema_de_tabelas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Heitor\Documents\Program\LumiTemp-ProjectBasedLearning\modelagem_banco_de_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986A4DC5-F885-40AE-B004-178E14E9FB25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCCA665-3159-44C0-8DAF-E31FACE8DF70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="11655" xr2:uid="{39708544-CF50-4C3E-BEB5-6B41EA60E03B}"/>
+    <workbookView xWindow="7200" yWindow="0" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{39708544-CF50-4C3E-BEB5-6B41EA60E03B}"/>
   </bookViews>
   <sheets>
     <sheet name="cadr_func" sheetId="2" r:id="rId1"/>
@@ -58,9 +58,6 @@
     <t>DATE</t>
   </si>
   <si>
-    <t>NR_USUA</t>
-  </si>
-  <si>
     <t>LOGIN</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
     <t>CD_MOTOR</t>
   </si>
   <si>
-    <t>FK_NR_USUA</t>
-  </si>
-  <si>
     <t>FK_CD_EMPR</t>
   </si>
   <si>
@@ -182,6 +176,12 @@
   </si>
   <si>
     <t>Telefone da empresa parceira</t>
+  </si>
+  <si>
+    <t>CD_FUNC</t>
+  </si>
+  <si>
+    <t>FK_CD_USUA</t>
   </si>
 </sst>
 </file>
@@ -603,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F5F82A-ED2B-4CA8-ACB4-71B7DD84976E}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,78 +627,78 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -710,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E25D063-F717-42E8-A840-E558CF89DBA5}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,180 +733,180 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -919,7 +919,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,112 +942,112 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inserindo procedures, corrigindo campos e redocumentando itens no sistema do banco de dados | 24.10.2024
</commit_message>
<xml_diff>
--- a/modelagem_banco_de_dados/esquema_de_tabelas.xlsx
+++ b/modelagem_banco_de_dados/esquema_de_tabelas.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Heitor\Documents\Program\LumiTemp-ProjectBasedLearning\modelagem_banco_de_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCCA665-3159-44C0-8DAF-E31FACE8DF70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D56D828-8D3A-4BD6-BDE5-8C3C716DB2E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="0" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{39708544-CF50-4C3E-BEB5-6B41EA60E03B}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15750" activeTab="2" xr2:uid="{39708544-CF50-4C3E-BEB5-6B41EA60E03B}"/>
   </bookViews>
   <sheets>
     <sheet name="cadr_func" sheetId="2" r:id="rId1"/>
-    <sheet name="sens_info" sheetId="1" r:id="rId2"/>
-    <sheet name="cadr_empr_parc" sheetId="3" r:id="rId3"/>
+    <sheet name="cadr_empr_parc" sheetId="3" r:id="rId2"/>
+    <sheet name="sens_info" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="40">
   <si>
     <t>Nome do campo</t>
   </si>
@@ -58,12 +58,6 @@
     <t>DATE</t>
   </si>
   <si>
-    <t>LOGIN</t>
-  </si>
-  <si>
-    <t>SENHA</t>
-  </si>
-  <si>
     <t>DT_CADR</t>
   </si>
   <si>
@@ -91,33 +85,15 @@
     <t>Foreing Key</t>
   </si>
   <si>
-    <t>CD_SENS</t>
-  </si>
-  <si>
     <t>DS_TIPO_SENS</t>
   </si>
   <si>
-    <t>DT_HR_LEIT</t>
-  </si>
-  <si>
-    <t>VL_TEMP</t>
-  </si>
-  <si>
-    <t>VL_UMID</t>
-  </si>
-  <si>
     <t>VL_TEMP_ALVO</t>
   </si>
   <si>
-    <t>VL_UMID_ALVO</t>
-  </si>
-  <si>
     <t>CD_MOTOR</t>
   </si>
   <si>
-    <t>FK_CD_EMPR</t>
-  </si>
-  <si>
     <t>DECIMAL</t>
   </si>
   <si>
@@ -133,15 +109,6 @@
     <t>Valor lido da temperatura</t>
   </si>
   <si>
-    <t>Valor lido da umidade</t>
-  </si>
-  <si>
-    <t>Valor alvo de temperatura</t>
-  </si>
-  <si>
-    <t>Valor alvo de umidade</t>
-  </si>
-  <si>
     <t>Código do motor que está sendo feita a leitura</t>
   </si>
   <si>
@@ -151,9 +118,6 @@
     <t>Código da empresa da qual o sensor está alocado/vendido</t>
   </si>
   <si>
-    <t>CD_EMPR</t>
-  </si>
-  <si>
     <t>NM_EMPR</t>
   </si>
   <si>
@@ -178,10 +142,22 @@
     <t>Telefone da empresa parceira</t>
   </si>
   <si>
-    <t>CD_FUNC</t>
-  </si>
-  <si>
-    <t>FK_CD_USUA</t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>LOGIN_FUNC</t>
+  </si>
+  <si>
+    <t>SENHA_FUNC</t>
+  </si>
+  <si>
+    <t>ID_FUNC</t>
+  </si>
+  <si>
+    <t>DT_VEND</t>
+  </si>
+  <si>
+    <t>ID_EMPR</t>
   </si>
 </sst>
 </file>
@@ -604,7 +580,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,78 +603,78 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -707,219 +683,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E25D063-F717-42E8-A840-E558CF89DBA5}">
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="93.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E92DA6-55AA-46C5-9317-2ED68382806A}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,112 +710,269 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E25D063-F717-42E8-A840-E558CF89DBA5}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>